<commit_message>
* fixed the generate report for all button - does not use multithreading now + GUI improvements
</commit_message>
<xml_diff>
--- a/templates/dev_templates/starter_template_copy.xlsx
+++ b/templates/dev_templates/starter_template_copy.xlsx
@@ -17,7 +17,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -59,6 +59,12 @@
       <color theme="4" tint="-0.249977111117893"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <family val="2"/>
+      <color indexed="81"/>
+      <sz val="9"/>
     </font>
   </fonts>
   <fills count="4">
@@ -219,43 +225,15 @@
 <file path=xl/comments/comment1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author>Owner</author>
+    <author>tc={488C16CC-3FD7-4363-B639-F87056FF341A}</author>
   </authors>
   <commentList>
-    <comment ref="E5" authorId="0" shapeId="0">
+    <comment ref="F5" authorId="0" shapeId="0">
       <text>
-        <t>Owner:
-Information attributed to the specific equipment. This will be stored in the database if indicated using the software</t>
-      </text>
-    </comment>
-    <comment ref="J5" authorId="0" shapeId="0">
-      <text>
-        <t>Owner:
-Importance factor.</t>
-      </text>
-    </comment>
-    <comment ref="M5" authorId="0" shapeId="0">
-      <text>
-        <t>Owner:
-Equipment width per diagram.</t>
-      </text>
-    </comment>
-    <comment ref="N5" authorId="0" shapeId="0">
-      <text>
-        <t>Owner:
-Equipment depth per diagram.</t>
-      </text>
-    </comment>
-    <comment ref="O5" authorId="0" shapeId="0">
-      <text>
-        <t>Owner:
-Distance from edge of equipment to mounting location along width axis per diagram.</t>
-      </text>
-    </comment>
-    <comment ref="P5" authorId="0" shapeId="0">
-      <text>
-        <t>Owner:
-Distance from edge of equipment to mounting location along depth axis per diagram.</t>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    this is the wb input</t>
       </text>
     </comment>
   </commentList>
@@ -734,8 +712,8 @@
   </sheetPr>
   <dimension ref="A1:S823"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.3"/>
@@ -912,7 +890,7 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>335</t>
+          <t>333</t>
         </is>
       </c>
       <c r="G6" t="n">

</xml_diff>

<commit_message>
+ added equipment tags category/input
</commit_message>
<xml_diff>
--- a/templates/dev_templates/starter_template_copy.xlsx
+++ b/templates/dev_templates/starter_template_copy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Desktop\mathcad_auto\templates\dev_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{619DCB4F-ADA6-4133-8295-6A74416C5487}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA1D66BB-0B9C-439A-B4F0-400DB0B97A59}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-109" yWindow="-109" windowWidth="34995" windowHeight="19196" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
     <author>tc={0DC467EE-0F37-418F-BA64-4FC751C4C3C3}</author>
   </authors>
   <commentList>
-    <comment ref="F5" authorId="0" shapeId="0" xr:uid="{0DC467EE-0F37-418F-BA64-4FC751C4C3C3}">
+    <comment ref="G5" authorId="0" shapeId="0" xr:uid="{0DC467EE-0F37-418F-BA64-4FC751C4C3C3}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="43">
   <si>
     <t xml:space="preserve">Mathcad Automation Template </t>
   </si>
@@ -153,6 +153,21 @@
   </si>
   <si>
     <t>ceiling</t>
+  </si>
+  <si>
+    <t>eqpt_tags</t>
+  </si>
+  <si>
+    <t>foo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Foo, Bar </t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Foo, Bar, A </t>
   </si>
 </sst>
 </file>
@@ -801,7 +816,7 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="F5" dT="2021-08-05T16:18:47.51" personId="{9240EDB1-4457-486C-BE4E-7811985DDED9}" id="{0DC467EE-0F37-418F-BA64-4FC751C4C3C3}">
+  <threadedComment ref="G5" dT="2021-08-05T16:18:47.51" personId="{9240EDB1-4457-486C-BE4E-7811985DDED9}" id="{0DC467EE-0F37-418F-BA64-4FC751C4C3C3}">
     <text>W_p input. The units are pounds adsfsdfasdfasdfasdfasdfasdfasdf</text>
   </threadedComment>
 </ThreadedComments>
@@ -809,55 +824,55 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S823"/>
+  <dimension ref="A1:T823"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I30" sqref="I30"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="32.125" style="1" customWidth="1"/>
-    <col min="3" max="4" width="25.125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="21.75" style="1" customWidth="1"/>
-    <col min="6" max="6" width="17.25" style="1" customWidth="1"/>
-    <col min="7" max="7" width="15.25" style="1" customWidth="1"/>
-    <col min="8" max="8" width="16.875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="14.75" style="1" customWidth="1"/>
-    <col min="10" max="10" width="15.125" style="1" customWidth="1"/>
-    <col min="11" max="12" width="9" style="1" customWidth="1"/>
-    <col min="13" max="13" width="16.75" style="1" customWidth="1"/>
-    <col min="14" max="14" width="16.625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="17.25" style="1" customWidth="1"/>
-    <col min="16" max="16" width="14.25" style="1" customWidth="1"/>
-    <col min="17" max="17" width="17.75" style="1" customWidth="1"/>
-    <col min="18" max="18" width="15.375" style="1" customWidth="1"/>
-    <col min="19" max="19" width="18.25" customWidth="1"/>
+    <col min="3" max="5" width="25.125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="21.75" style="1" customWidth="1"/>
+    <col min="7" max="7" width="17.25" style="1" customWidth="1"/>
+    <col min="8" max="8" width="15.25" style="1" customWidth="1"/>
+    <col min="9" max="9" width="16.875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="14.75" style="1" customWidth="1"/>
+    <col min="11" max="11" width="15.125" style="1" customWidth="1"/>
+    <col min="12" max="13" width="9" style="1" customWidth="1"/>
+    <col min="14" max="14" width="16.75" style="1" customWidth="1"/>
+    <col min="15" max="15" width="16.625" style="1" customWidth="1"/>
+    <col min="16" max="16" width="17.25" style="1" customWidth="1"/>
+    <col min="17" max="17" width="14.25" style="1" customWidth="1"/>
+    <col min="18" max="18" width="17.75" style="1" customWidth="1"/>
+    <col min="19" max="19" width="15.375" style="1" customWidth="1"/>
+    <col min="20" max="20" width="18.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="21.1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:20" ht="21.1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2"/>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:19" ht="14.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:20" ht="14.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
@@ -871,52 +886,55 @@
         <v>8</v>
       </c>
       <c r="E5" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="G5" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="H5" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="H5" s="5" t="s">
+      <c r="I5" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="I5" s="5" t="s">
+      <c r="J5" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="J5" s="5" t="s">
+      <c r="K5" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="K5" s="5" t="s">
+      <c r="L5" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="L5" s="5" t="s">
+      <c r="M5" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="M5" s="5" t="s">
+      <c r="N5" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="N5" s="5" t="s">
+      <c r="O5" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="O5" s="5" t="s">
+      <c r="P5" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="P5" s="5" t="s">
+      <c r="Q5" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="Q5" s="5" t="s">
+      <c r="R5" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="R5" s="5" t="s">
+      <c r="S5" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="S5" s="5" t="s">
+      <c r="T5" s="5" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>24</v>
       </c>
@@ -930,52 +948,55 @@
         <v>1111</v>
       </c>
       <c r="E6" t="s">
+        <v>39</v>
+      </c>
+      <c r="F6" t="s">
         <v>26</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>27</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>1.121</v>
       </c>
-      <c r="H6">
+      <c r="I6">
         <v>1</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <v>2.5</v>
       </c>
-      <c r="J6">
+      <c r="K6">
         <v>1.5</v>
       </c>
-      <c r="K6">
+      <c r="L6">
         <v>0</v>
       </c>
-      <c r="L6">
+      <c r="M6">
         <v>75</v>
       </c>
-      <c r="M6">
+      <c r="N6">
         <v>30</v>
       </c>
-      <c r="N6">
+      <c r="O6">
         <v>20.5</v>
       </c>
-      <c r="O6">
+      <c r="P6">
         <v>1.5</v>
       </c>
-      <c r="P6">
+      <c r="Q6">
         <v>-1.5</v>
       </c>
-      <c r="Q6">
+      <c r="R6">
         <v>74.25</v>
       </c>
-      <c r="R6">
+      <c r="S6">
         <v>2.5</v>
       </c>
-      <c r="S6">
+      <c r="T6">
         <v>0.66666599999999998</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>28</v>
       </c>
@@ -989,52 +1010,55 @@
         <v>1111</v>
       </c>
       <c r="E7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F7" t="s">
         <v>29</v>
       </c>
-      <c r="F7">
+      <c r="G7">
         <v>137</v>
       </c>
-      <c r="G7">
+      <c r="H7">
         <v>1.121</v>
       </c>
-      <c r="H7">
+      <c r="I7">
         <v>1</v>
       </c>
-      <c r="I7">
+      <c r="J7">
         <v>2.5</v>
       </c>
-      <c r="J7">
+      <c r="K7">
         <v>1.5</v>
       </c>
-      <c r="K7">
+      <c r="L7">
         <v>3</v>
       </c>
-      <c r="L7">
+      <c r="M7">
         <v>75</v>
       </c>
-      <c r="M7">
+      <c r="N7">
         <v>30</v>
       </c>
-      <c r="N7">
+      <c r="O7">
         <v>21.5</v>
       </c>
-      <c r="O7">
+      <c r="P7">
         <v>1.5</v>
       </c>
-      <c r="P7">
+      <c r="Q7">
         <v>-3.5</v>
       </c>
-      <c r="Q7">
+      <c r="R7">
         <v>24.5</v>
       </c>
-      <c r="R7">
+      <c r="S7">
         <v>2.5</v>
       </c>
-      <c r="S7">
+      <c r="T7">
         <v>0.66666599999999998</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>30</v>
       </c>
@@ -1048,52 +1072,55 @@
         <v>1111</v>
       </c>
       <c r="E8" t="s">
+        <v>41</v>
+      </c>
+      <c r="F8" t="s">
         <v>29</v>
       </c>
-      <c r="F8">
+      <c r="G8">
         <v>295</v>
       </c>
-      <c r="G8">
+      <c r="H8">
         <v>1.121</v>
       </c>
-      <c r="H8">
+      <c r="I8">
         <v>1</v>
       </c>
-      <c r="I8">
+      <c r="J8">
         <v>2.5</v>
       </c>
-      <c r="J8">
+      <c r="K8">
         <v>1.5</v>
       </c>
-      <c r="K8">
+      <c r="L8">
         <v>4</v>
       </c>
-      <c r="L8">
+      <c r="M8">
         <v>75</v>
       </c>
-      <c r="M8">
+      <c r="N8">
         <v>64</v>
       </c>
-      <c r="N8">
+      <c r="O8">
         <v>28</v>
       </c>
-      <c r="O8">
+      <c r="P8">
         <v>1.5</v>
       </c>
-      <c r="P8">
+      <c r="Q8">
         <v>-3.5</v>
       </c>
-      <c r="Q8">
+      <c r="R8">
         <v>39.5</v>
       </c>
-      <c r="R8">
+      <c r="S8">
         <v>2.5</v>
       </c>
-      <c r="S8">
+      <c r="T8">
         <v>0.66666599999999998</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>31</v>
       </c>
@@ -1107,46 +1134,49 @@
         <v>1111</v>
       </c>
       <c r="E9" t="s">
+        <v>42</v>
+      </c>
+      <c r="F9" t="s">
         <v>29</v>
       </c>
-      <c r="F9">
+      <c r="G9">
         <v>800</v>
       </c>
-      <c r="G9">
+      <c r="H9">
         <v>1.121</v>
       </c>
-      <c r="H9">
+      <c r="I9">
         <v>1</v>
       </c>
-      <c r="I9">
+      <c r="J9">
         <v>2.5</v>
       </c>
-      <c r="J9">
+      <c r="K9">
         <v>1.5</v>
       </c>
-      <c r="K9">
+      <c r="L9">
         <v>15</v>
       </c>
-      <c r="L9">
+      <c r="M9">
         <v>75</v>
-      </c>
-      <c r="O9">
-        <v>14</v>
       </c>
       <c r="P9">
         <v>14</v>
       </c>
       <c r="Q9">
+        <v>14</v>
+      </c>
+      <c r="R9">
         <v>45</v>
       </c>
-      <c r="R9">
+      <c r="S9">
         <v>2.5</v>
       </c>
-      <c r="S9">
+      <c r="T9">
         <v>0.66666599999999998</v>
       </c>
     </row>
-    <row r="823" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="823" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A823" s="4"/>
       <c r="B823" s="4"/>
       <c r="C823" s="4"/>
@@ -1166,6 +1196,7 @@
       <c r="Q823" s="4"/>
       <c r="R823" s="4"/>
       <c r="S823" s="4"/>
+      <c r="T823" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>